<commit_message>
Added in MIT licence (limits liability and warranty, allows re-use including commercial under the condition that licence and copyright notice are retained)
</commit_message>
<xml_diff>
--- a/process/_project_configuration.xlsx
+++ b/process/_project_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ind_bangkok\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF77A966-FBD0-42A7-BC60-1B615709F6A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D28E607-3949-4F2E-8A6D-E86DB064155A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="29" r:id="rId1"/>
@@ -8699,7 +8699,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9279,66 +9279,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -9372,11 +9312,68 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -10959,8 +10956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B626DB50-8A0C-462F-BEDD-A2065F5D6894}">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10970,11 +10967,11 @@
     <col min="3" max="3" width="107.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="241" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
+    <row r="1" spans="1:3" s="221" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="242" t="s">
         <v>2124</v>
       </c>
-      <c r="B1" s="243"/>
+      <c r="B1" s="242"/>
       <c r="C1" s="242"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -11017,11 +11014,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="240" t="s">
+      <c r="A12" s="220" t="s">
         <v>2119</v>
       </c>
       <c r="B12" s="86"/>
-      <c r="C12" s="239" t="s">
+      <c r="C12" s="219" t="s">
         <v>2118</v>
       </c>
     </row>
@@ -11034,12 +11031,12 @@
       <c r="A14" s="17" t="s">
         <v>2117</v>
       </c>
-      <c r="C14" s="238" t="s">
+      <c r="C14" s="218" t="s">
         <v>2116</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="237" t="s">
+      <c r="B15" s="217" t="s">
         <v>1313</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -11047,7 +11044,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="237" t="s">
+      <c r="B16" s="217" t="s">
         <v>2114</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -11055,7 +11052,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="237" t="s">
+      <c r="B17" s="217" t="s">
         <v>2112</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -11063,7 +11060,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="237" t="s">
+      <c r="B18" s="217" t="s">
         <v>2110</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -11071,7 +11068,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="237" t="s">
+      <c r="B19" s="217" t="s">
         <v>2108</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -11079,7 +11076,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="237" t="s">
+      <c r="B20" s="217" t="s">
         <v>1325</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -11106,7 +11103,7 @@
       <c r="C23" s="90"/>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="235" t="s">
+      <c r="A24" s="215" t="s">
         <v>2103</v>
       </c>
       <c r="B24" s="18"/>
@@ -11115,19 +11112,19 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="235"/>
+      <c r="A25" s="215"/>
       <c r="B25" s="16"/>
       <c r="C25" s="6" t="s">
         <v>2102</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="236"/>
+      <c r="A26" s="216"/>
       <c r="B26" s="89"/>
       <c r="C26" s="90"/>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="235" t="s">
+      <c r="A27" s="215" t="s">
         <v>2101</v>
       </c>
       <c r="B27" s="18"/>
@@ -11564,6 +11561,9 @@
       <c r="C88" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <conditionalFormatting sqref="B15:B20">
     <cfRule type="expression" dxfId="167" priority="1">
       <formula>OR(ISERR(FIND("Requires", $B15))=FALSE,ISERR(FIND("Could", $T15))=FALSE)</formula>
@@ -11614,32 +11614,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="232" t="s">
         <v>1290</v>
       </c>
-      <c r="B1" s="211"/>
-      <c r="C1" s="211"/>
-      <c r="D1" s="211"/>
+      <c r="B1" s="232"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232"/>
       <c r="E1" s="33"/>
-      <c r="F1" s="212" t="s">
+      <c r="F1" s="233" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="213" t="s">
+      <c r="G1" s="233"/>
+      <c r="H1" s="233"/>
+      <c r="I1" s="234" t="s">
         <v>1500</v>
       </c>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="213"/>
-      <c r="N1" s="213"/>
-      <c r="O1" s="213"/>
-      <c r="P1" s="213"/>
-      <c r="Q1" s="213"/>
-      <c r="R1" s="213"/>
-      <c r="S1" s="213"/>
-      <c r="T1" s="213"/>
+      <c r="J1" s="234"/>
+      <c r="K1" s="234"/>
+      <c r="L1" s="234"/>
+      <c r="M1" s="234"/>
+      <c r="N1" s="234"/>
+      <c r="O1" s="234"/>
+      <c r="P1" s="234"/>
+      <c r="Q1" s="234"/>
+      <c r="R1" s="234"/>
+      <c r="S1" s="234"/>
+      <c r="T1" s="234"/>
     </row>
     <row r="2" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="106" t="s">
@@ -11648,10 +11648,10 @@
       <c r="B2" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="214" t="s">
+      <c r="C2" s="235" t="s">
         <v>1501</v>
       </c>
-      <c r="D2" s="214"/>
+      <c r="D2" s="235"/>
       <c r="E2" s="135" t="s">
         <v>1279</v>
       </c>
@@ -11664,23 +11664,23 @@
       <c r="H2" s="135" t="s">
         <v>1997</v>
       </c>
-      <c r="I2" s="214" t="s">
+      <c r="I2" s="235" t="s">
         <v>1504</v>
       </c>
-      <c r="J2" s="214"/>
-      <c r="K2" s="214"/>
+      <c r="J2" s="235"/>
+      <c r="K2" s="235"/>
       <c r="L2" s="205"/>
-      <c r="M2" s="214" t="s">
+      <c r="M2" s="235" t="s">
         <v>1505</v>
       </c>
-      <c r="N2" s="214"/>
-      <c r="O2" s="214"/>
+      <c r="N2" s="235"/>
+      <c r="O2" s="235"/>
       <c r="P2" s="205"/>
-      <c r="Q2" s="215" t="s">
+      <c r="Q2" s="236" t="s">
         <v>1506</v>
       </c>
-      <c r="R2" s="215"/>
-      <c r="S2" s="215"/>
+      <c r="R2" s="236"/>
+      <c r="S2" s="236"/>
       <c r="T2" s="105"/>
     </row>
     <row r="3" spans="1:20" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -11730,17 +11730,17 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="216">
+      <c r="A4" s="222">
         <v>1</v>
       </c>
-      <c r="B4" s="219" t="s">
+      <c r="B4" s="225" t="s">
         <v>1298</v>
       </c>
-      <c r="C4" s="219" t="str">
+      <c r="C4" s="225" t="str">
         <f>SUM(S4:S10)&amp;"/"&amp;SUM(R4:R10)</f>
         <v>22/22</v>
       </c>
-      <c r="D4" s="222">
+      <c r="D4" s="229">
         <f>SUM(S4:S10)/SUM(R4:R10)</f>
         <v>1</v>
       </c>
@@ -11800,10 +11800,10 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="217"/>
-      <c r="B5" s="220"/>
-      <c r="C5" s="220"/>
-      <c r="D5" s="223"/>
+      <c r="A5" s="223"/>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="230"/>
       <c r="E5" s="147">
         <v>2</v>
       </c>
@@ -11860,10 +11860,10 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="217"/>
-      <c r="B6" s="220"/>
-      <c r="C6" s="220"/>
-      <c r="D6" s="223"/>
+      <c r="A6" s="223"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="230"/>
       <c r="E6" s="147">
         <v>3</v>
       </c>
@@ -11920,10 +11920,10 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="217"/>
-      <c r="B7" s="220"/>
-      <c r="C7" s="220"/>
-      <c r="D7" s="223"/>
+      <c r="A7" s="223"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="230"/>
       <c r="E7" s="147">
         <v>4</v>
       </c>
@@ -11980,10 +11980,10 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="217"/>
-      <c r="B8" s="220"/>
-      <c r="C8" s="220"/>
-      <c r="D8" s="223"/>
+      <c r="A8" s="223"/>
+      <c r="B8" s="226"/>
+      <c r="C8" s="226"/>
+      <c r="D8" s="230"/>
       <c r="E8" s="147">
         <v>5</v>
       </c>
@@ -12040,10 +12040,10 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="217"/>
-      <c r="B9" s="220"/>
-      <c r="C9" s="220"/>
-      <c r="D9" s="223"/>
+      <c r="A9" s="223"/>
+      <c r="B9" s="226"/>
+      <c r="C9" s="226"/>
+      <c r="D9" s="230"/>
       <c r="E9" s="147">
         <v>6</v>
       </c>
@@ -12100,10 +12100,10 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="218"/>
-      <c r="B10" s="221"/>
-      <c r="C10" s="221"/>
-      <c r="D10" s="224"/>
+      <c r="A10" s="224"/>
+      <c r="B10" s="227"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="231"/>
       <c r="E10" s="152">
         <v>7</v>
       </c>
@@ -12160,17 +12160,17 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="216">
+      <c r="A11" s="222">
         <v>2</v>
       </c>
-      <c r="B11" s="219" t="s">
+      <c r="B11" s="225" t="s">
         <v>1376</v>
       </c>
-      <c r="C11" s="219" t="str">
+      <c r="C11" s="225" t="str">
         <f>SUM(S11:S14)&amp;"/"&amp;SUM(R11:R14)</f>
         <v>13/13</v>
       </c>
-      <c r="D11" s="225">
+      <c r="D11" s="228">
         <f>SUM(S11:S14)/SUM(R11:R14)</f>
         <v>1</v>
       </c>
@@ -12230,10 +12230,10 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="217"/>
-      <c r="B12" s="220"/>
-      <c r="C12" s="220"/>
-      <c r="D12" s="220"/>
+      <c r="A12" s="223"/>
+      <c r="B12" s="226"/>
+      <c r="C12" s="226"/>
+      <c r="D12" s="226"/>
       <c r="E12" s="147">
         <v>9</v>
       </c>
@@ -12290,10 +12290,10 @@
       </c>
     </row>
     <row r="13" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="217"/>
-      <c r="B13" s="220"/>
-      <c r="C13" s="220"/>
-      <c r="D13" s="220"/>
+      <c r="A13" s="223"/>
+      <c r="B13" s="226"/>
+      <c r="C13" s="226"/>
+      <c r="D13" s="226"/>
       <c r="E13" s="147">
         <v>10</v>
       </c>
@@ -12350,10 +12350,10 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="218"/>
-      <c r="B14" s="221"/>
-      <c r="C14" s="221"/>
-      <c r="D14" s="221"/>
+      <c r="A14" s="224"/>
+      <c r="B14" s="227"/>
+      <c r="C14" s="227"/>
+      <c r="D14" s="227"/>
       <c r="E14" s="152">
         <v>11</v>
       </c>
@@ -12410,17 +12410,17 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="216">
+      <c r="A15" s="222">
         <v>3</v>
       </c>
-      <c r="B15" s="219" t="s">
+      <c r="B15" s="225" t="s">
         <v>1410</v>
       </c>
-      <c r="C15" s="219" t="str">
+      <c r="C15" s="225" t="str">
         <f>SUM(S15:S22)&amp;"/"&amp;SUM(R15:R22)</f>
         <v>22/22</v>
       </c>
-      <c r="D15" s="225">
+      <c r="D15" s="228">
         <f>SUM(S15:S22)/SUM(R15:R22)</f>
         <v>1</v>
       </c>
@@ -12480,10 +12480,10 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="217"/>
-      <c r="B16" s="220"/>
-      <c r="C16" s="220"/>
-      <c r="D16" s="220"/>
+      <c r="A16" s="223"/>
+      <c r="B16" s="226"/>
+      <c r="C16" s="226"/>
+      <c r="D16" s="226"/>
       <c r="E16" s="147">
         <v>13</v>
       </c>
@@ -12540,10 +12540,10 @@
       </c>
     </row>
     <row r="17" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="217"/>
-      <c r="B17" s="220"/>
-      <c r="C17" s="220"/>
-      <c r="D17" s="220"/>
+      <c r="A17" s="223"/>
+      <c r="B17" s="226"/>
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
       <c r="E17" s="147">
         <v>14</v>
       </c>
@@ -12600,10 +12600,10 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="217"/>
-      <c r="B18" s="220"/>
-      <c r="C18" s="220"/>
-      <c r="D18" s="220"/>
+      <c r="A18" s="223"/>
+      <c r="B18" s="226"/>
+      <c r="C18" s="226"/>
+      <c r="D18" s="226"/>
       <c r="E18" s="147">
         <v>15</v>
       </c>
@@ -12660,10 +12660,10 @@
       </c>
     </row>
     <row r="19" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="217"/>
-      <c r="B19" s="220"/>
-      <c r="C19" s="220"/>
-      <c r="D19" s="220"/>
+      <c r="A19" s="223"/>
+      <c r="B19" s="226"/>
+      <c r="C19" s="226"/>
+      <c r="D19" s="226"/>
       <c r="E19" s="147">
         <v>16</v>
       </c>
@@ -12720,10 +12720,10 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="217"/>
-      <c r="B20" s="220"/>
-      <c r="C20" s="220"/>
-      <c r="D20" s="220"/>
+      <c r="A20" s="223"/>
+      <c r="B20" s="226"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="226"/>
       <c r="E20" s="147">
         <v>17</v>
       </c>
@@ -12780,10 +12780,10 @@
       </c>
     </row>
     <row r="21" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="217"/>
-      <c r="B21" s="220"/>
-      <c r="C21" s="220"/>
-      <c r="D21" s="220"/>
+      <c r="A21" s="223"/>
+      <c r="B21" s="226"/>
+      <c r="C21" s="226"/>
+      <c r="D21" s="226"/>
       <c r="E21" s="147">
         <v>18</v>
       </c>
@@ -12840,10 +12840,10 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="218"/>
-      <c r="B22" s="221"/>
-      <c r="C22" s="221"/>
-      <c r="D22" s="221"/>
+      <c r="A22" s="224"/>
+      <c r="B22" s="227"/>
+      <c r="C22" s="227"/>
+      <c r="D22" s="227"/>
       <c r="E22" s="152">
         <v>19</v>
       </c>
@@ -12900,17 +12900,17 @@
       </c>
     </row>
     <row r="23" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="216">
+      <c r="A23" s="222">
         <v>4</v>
       </c>
-      <c r="B23" s="219" t="s">
+      <c r="B23" s="225" t="s">
         <v>1474</v>
       </c>
-      <c r="C23" s="219" t="str">
+      <c r="C23" s="225" t="str">
         <f>SUM(S23:S27)&amp;"/"&amp;SUM(R23:R27)</f>
         <v>3/3</v>
       </c>
-      <c r="D23" s="225">
+      <c r="D23" s="228">
         <f>SUM(S23:S27)/SUM(R23:R27)</f>
         <v>1</v>
       </c>
@@ -12970,10 +12970,10 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="217"/>
-      <c r="B24" s="220"/>
-      <c r="C24" s="220"/>
-      <c r="D24" s="220"/>
+      <c r="A24" s="223"/>
+      <c r="B24" s="226"/>
+      <c r="C24" s="226"/>
+      <c r="D24" s="226"/>
       <c r="E24" s="147">
         <v>21</v>
       </c>
@@ -13030,10 +13030,10 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="217"/>
-      <c r="B25" s="220"/>
-      <c r="C25" s="220"/>
-      <c r="D25" s="220"/>
+      <c r="A25" s="223"/>
+      <c r="B25" s="226"/>
+      <c r="C25" s="226"/>
+      <c r="D25" s="226"/>
       <c r="E25" s="147">
         <v>22</v>
       </c>
@@ -13090,10 +13090,10 @@
       </c>
     </row>
     <row r="26" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="217"/>
-      <c r="B26" s="220"/>
-      <c r="C26" s="220"/>
-      <c r="D26" s="220"/>
+      <c r="A26" s="223"/>
+      <c r="B26" s="226"/>
+      <c r="C26" s="226"/>
+      <c r="D26" s="226"/>
       <c r="E26" s="147">
         <v>23</v>
       </c>
@@ -13150,10 +13150,10 @@
       </c>
     </row>
     <row r="27" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="218"/>
-      <c r="B27" s="221"/>
-      <c r="C27" s="221"/>
-      <c r="D27" s="221"/>
+      <c r="A27" s="224"/>
+      <c r="B27" s="227"/>
+      <c r="C27" s="227"/>
+      <c r="D27" s="227"/>
       <c r="E27" s="152">
         <v>24</v>
       </c>
@@ -13275,6 +13275,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:T1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="D4:D10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
     <mergeCell ref="A15:A22"/>
     <mergeCell ref="B15:B22"/>
     <mergeCell ref="C15:C22"/>
@@ -13283,21 +13298,6 @@
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="C23:C27"/>
     <mergeCell ref="D23:D27"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="D4:D10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:T1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="Q2:S2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:T27">
     <cfRule type="expression" dxfId="161" priority="2">
@@ -13369,31 +13369,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="226" t="s">
+      <c r="B1" s="237" t="s">
         <v>1283</v>
       </c>
-      <c r="C1" s="226"/>
+      <c r="C1" s="237"/>
       <c r="D1" s="112"/>
-      <c r="E1" s="226" t="s">
+      <c r="E1" s="237" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="226"/>
+      <c r="F1" s="237"/>
       <c r="G1" s="112"/>
-      <c r="H1" s="226" t="s">
+      <c r="H1" s="237" t="s">
         <v>1284</v>
       </c>
-      <c r="I1" s="226"/>
+      <c r="I1" s="237"/>
       <c r="J1" s="112" t="s">
         <v>1285</v>
       </c>
       <c r="K1" s="112"/>
-      <c r="L1" s="226" t="s">
+      <c r="L1" s="237" t="s">
         <v>288</v>
       </c>
-      <c r="M1" s="226"/>
-      <c r="N1" s="226"/>
-      <c r="O1" s="226"/>
-      <c r="P1" s="226"/>
+      <c r="M1" s="237"/>
+      <c r="N1" s="237"/>
+      <c r="O1" s="237"/>
+      <c r="P1" s="237"/>
       <c r="Q1" s="113"/>
       <c r="R1" s="113"/>
       <c r="S1" s="113"/>
@@ -13404,10 +13404,10 @@
         <v>1287</v>
       </c>
       <c r="V1" s="112"/>
-      <c r="W1" s="226" t="s">
+      <c r="W1" s="237" t="s">
         <v>1288</v>
       </c>
-      <c r="X1" s="226"/>
+      <c r="X1" s="237"/>
       <c r="Y1" s="112"/>
       <c r="Z1" s="112" t="s">
         <v>1289</v>
@@ -13436,11 +13436,11 @@
       </c>
       <c r="J2" s="115"/>
       <c r="K2" s="91"/>
-      <c r="L2" s="227" t="s">
+      <c r="L2" s="238" t="s">
         <v>1291</v>
       </c>
-      <c r="M2" s="227"/>
-      <c r="N2" s="227"/>
+      <c r="M2" s="238"/>
+      <c r="N2" s="238"/>
       <c r="O2" s="115"/>
       <c r="P2" s="115" t="s">
         <v>75</v>
@@ -13448,10 +13448,10 @@
       <c r="Q2" s="116" t="s">
         <v>1292</v>
       </c>
-      <c r="R2" s="228" t="s">
+      <c r="R2" s="239" t="s">
         <v>1293</v>
       </c>
-      <c r="S2" s="228" t="s">
+      <c r="S2" s="239" t="s">
         <v>1294</v>
       </c>
       <c r="T2" s="117"/>
@@ -13490,8 +13490,8 @@
       <c r="O3" s="105"/>
       <c r="P3" s="105"/>
       <c r="Q3" s="108"/>
-      <c r="R3" s="229"/>
-      <c r="S3" s="229"/>
+      <c r="R3" s="240"/>
+      <c r="S3" s="240"/>
       <c r="T3" s="122"/>
       <c r="U3" s="122"/>
       <c r="V3" s="118"/>
@@ -20423,64 +20423,64 @@
       <c r="F1" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="G1" s="226" t="s">
+      <c r="G1" s="237" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="226"/>
-      <c r="L1" s="226"/>
-      <c r="M1" s="226"/>
-      <c r="N1" s="226"/>
-      <c r="O1" s="226"/>
-      <c r="P1" s="226"/>
-      <c r="Q1" s="226"/>
-      <c r="R1" s="226"/>
-      <c r="S1" s="226"/>
-      <c r="T1" s="226"/>
-      <c r="U1" s="226"/>
-      <c r="V1" s="226"/>
-      <c r="W1" s="226"/>
-      <c r="X1" s="226"/>
-      <c r="Y1" s="226"/>
-      <c r="Z1" s="226"/>
-      <c r="AA1" s="226"/>
-      <c r="AB1" s="226"/>
-      <c r="AC1" s="226"/>
-      <c r="AD1" s="226"/>
-      <c r="AE1" s="226"/>
-      <c r="AF1" s="226"/>
-      <c r="AG1" s="226"/>
-      <c r="AH1" s="226"/>
-      <c r="AI1" s="226"/>
-      <c r="AJ1" s="226"/>
-      <c r="AK1" s="226"/>
-      <c r="AL1" s="226"/>
-      <c r="AM1" s="226"/>
-      <c r="AN1" s="226"/>
-      <c r="AO1" s="226"/>
-      <c r="AP1" s="226"/>
-      <c r="AQ1" s="226"/>
-      <c r="AR1" s="226"/>
-      <c r="AS1" s="226"/>
-      <c r="AT1" s="226"/>
-      <c r="AU1" s="226"/>
-      <c r="AV1" s="226"/>
-      <c r="AW1" s="226"/>
-      <c r="AX1" s="226"/>
-      <c r="AY1" s="226"/>
-      <c r="AZ1" s="226"/>
-      <c r="BA1" s="226"/>
-      <c r="BB1" s="226"/>
-      <c r="BC1" s="226"/>
-      <c r="BD1" s="226"/>
+      <c r="H1" s="237"/>
+      <c r="I1" s="237"/>
+      <c r="J1" s="237"/>
+      <c r="K1" s="237"/>
+      <c r="L1" s="237"/>
+      <c r="M1" s="237"/>
+      <c r="N1" s="237"/>
+      <c r="O1" s="237"/>
+      <c r="P1" s="237"/>
+      <c r="Q1" s="237"/>
+      <c r="R1" s="237"/>
+      <c r="S1" s="237"/>
+      <c r="T1" s="237"/>
+      <c r="U1" s="237"/>
+      <c r="V1" s="237"/>
+      <c r="W1" s="237"/>
+      <c r="X1" s="237"/>
+      <c r="Y1" s="237"/>
+      <c r="Z1" s="237"/>
+      <c r="AA1" s="237"/>
+      <c r="AB1" s="237"/>
+      <c r="AC1" s="237"/>
+      <c r="AD1" s="237"/>
+      <c r="AE1" s="237"/>
+      <c r="AF1" s="237"/>
+      <c r="AG1" s="237"/>
+      <c r="AH1" s="237"/>
+      <c r="AI1" s="237"/>
+      <c r="AJ1" s="237"/>
+      <c r="AK1" s="237"/>
+      <c r="AL1" s="237"/>
+      <c r="AM1" s="237"/>
+      <c r="AN1" s="237"/>
+      <c r="AO1" s="237"/>
+      <c r="AP1" s="237"/>
+      <c r="AQ1" s="237"/>
+      <c r="AR1" s="237"/>
+      <c r="AS1" s="237"/>
+      <c r="AT1" s="237"/>
+      <c r="AU1" s="237"/>
+      <c r="AV1" s="237"/>
+      <c r="AW1" s="237"/>
+      <c r="AX1" s="237"/>
+      <c r="AY1" s="237"/>
+      <c r="AZ1" s="237"/>
+      <c r="BA1" s="237"/>
+      <c r="BB1" s="237"/>
+      <c r="BC1" s="237"/>
+      <c r="BD1" s="237"/>
       <c r="BE1" s="9"/>
-      <c r="BH1" s="230" t="s">
+      <c r="BH1" s="241" t="s">
         <v>394</v>
       </c>
-      <c r="BI1" s="230"/>
-      <c r="BJ1" s="230"/>
+      <c r="BI1" s="241"/>
+      <c r="BJ1" s="241"/>
       <c r="BK1" s="62"/>
       <c r="BL1" s="82" t="s">
         <v>381</v>
@@ -41050,8 +41050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51613144-E587-4FFC-973B-724A2DE15856}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41060,7 +41060,7 @@
     <col min="2" max="4" width="32.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="84" style="6" customWidth="1"/>
     <col min="6" max="7" width="49.85546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="55.28515625" style="231" customWidth="1"/>
+    <col min="8" max="8" width="55.28515625" style="211" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -41084,7 +41084,7 @@
         <v>2050</v>
       </c>
       <c r="G1" s="19"/>
-      <c r="H1" s="234"/>
+      <c r="H1" s="214"/>
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -41099,8 +41099,8 @@
       <c r="F2" s="6" t="s">
         <v>2047</v>
       </c>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
+      <c r="G2" s="212"/>
+      <c r="H2" s="212"/>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -41109,7 +41109,7 @@
       <c r="B3" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C3" s="233" t="s">
+      <c r="C3" s="213" t="s">
         <v>2045</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -41121,8 +41121,8 @@
       <c r="F3" s="6" t="s">
         <v>2043</v>
       </c>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
+      <c r="G3" s="212"/>
+      <c r="H3" s="212"/>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
@@ -41131,7 +41131,7 @@
       <c r="B4" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C4" s="233" t="s">
+      <c r="C4" s="213" t="s">
         <v>2018</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -41143,8 +41143,8 @@
       <c r="F4" s="6" t="s">
         <v>2041</v>
       </c>
-      <c r="G4" s="232"/>
-      <c r="H4" s="232"/>
+      <c r="G4" s="212"/>
+      <c r="H4" s="212"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -41153,7 +41153,7 @@
       <c r="B5" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C5" s="233" t="s">
+      <c r="C5" s="213" t="s">
         <v>2018</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -41165,8 +41165,8 @@
       <c r="F5" s="6" t="s">
         <v>2040</v>
       </c>
-      <c r="G5" s="232"/>
-      <c r="H5" s="232"/>
+      <c r="G5" s="212"/>
+      <c r="H5" s="212"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -41175,7 +41175,7 @@
       <c r="B6" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C6" s="233" t="s">
+      <c r="C6" s="213" t="s">
         <v>2038</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -41187,8 +41187,8 @@
       <c r="F6" s="6" t="s">
         <v>2036</v>
       </c>
-      <c r="G6" s="232"/>
-      <c r="H6" s="232"/>
+      <c r="G6" s="212"/>
+      <c r="H6" s="212"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
@@ -41209,8 +41209,8 @@
       <c r="F7" s="6" t="s">
         <v>2031</v>
       </c>
-      <c r="G7" s="232"/>
-      <c r="H7" s="232"/>
+      <c r="G7" s="212"/>
+      <c r="H7" s="212"/>
     </row>
     <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -41219,7 +41219,7 @@
       <c r="B8" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C8" s="233" t="s">
+      <c r="C8" s="213" t="s">
         <v>2018</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -41231,8 +41231,8 @@
       <c r="F8" s="6" t="s">
         <v>2028</v>
       </c>
-      <c r="G8" s="232"/>
-      <c r="H8" s="232"/>
+      <c r="G8" s="212"/>
+      <c r="H8" s="212"/>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
@@ -41241,7 +41241,7 @@
       <c r="B9" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C9" s="233" t="s">
+      <c r="C9" s="213" t="s">
         <v>2018</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -41253,8 +41253,8 @@
       <c r="F9" s="6" t="s">
         <v>2025</v>
       </c>
-      <c r="G9" s="232"/>
-      <c r="H9" s="232"/>
+      <c r="G9" s="212"/>
+      <c r="H9" s="212"/>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -41263,7 +41263,7 @@
       <c r="B10" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C10" s="233" t="s">
+      <c r="C10" s="213" t="s">
         <v>2018</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -41275,8 +41275,8 @@
       <c r="F10" s="6" t="s">
         <v>2022</v>
       </c>
-      <c r="G10" s="232"/>
-      <c r="H10" s="232"/>
+      <c r="G10" s="212"/>
+      <c r="H10" s="212"/>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
@@ -41291,8 +41291,8 @@
       <c r="F11" s="6" t="s">
         <v>2019</v>
       </c>
-      <c r="G11" s="232"/>
-      <c r="H11" s="232"/>
+      <c r="G11" s="212"/>
+      <c r="H11" s="212"/>
     </row>
     <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
@@ -41301,7 +41301,7 @@
       <c r="B12" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C12" s="233" t="s">
+      <c r="C12" s="213" t="s">
         <v>2018</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -41313,8 +41313,8 @@
       <c r="F12" s="6" t="s">
         <v>2016</v>
       </c>
-      <c r="G12" s="232"/>
-      <c r="H12" s="232"/>
+      <c r="G12" s="212"/>
+      <c r="H12" s="212"/>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
@@ -41323,7 +41323,7 @@
       <c r="B13" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C13" s="233"/>
+      <c r="C13" s="213"/>
       <c r="D13" s="4" t="s">
         <v>2015</v>
       </c>
@@ -41333,8 +41333,8 @@
       <c r="F13" s="6" t="s">
         <v>2013</v>
       </c>
-      <c r="G13" s="232"/>
-      <c r="H13" s="232"/>
+      <c r="G13" s="212"/>
+      <c r="H13" s="212"/>
     </row>
     <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -41355,8 +41355,8 @@
       <c r="F14" s="6" t="s">
         <v>2009</v>
       </c>
-      <c r="G14" s="232"/>
-      <c r="H14" s="232"/>
+      <c r="G14" s="212"/>
+      <c r="H14" s="212"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
@@ -41365,7 +41365,7 @@
       <c r="B15" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C15" s="233" t="s">
+      <c r="C15" s="213" t="s">
         <v>2007</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -41377,8 +41377,8 @@
       <c r="F15" s="6" t="s">
         <v>2004</v>
       </c>
-      <c r="G15" s="232"/>
-      <c r="H15" s="232"/>
+      <c r="G15" s="212"/>
+      <c r="H15" s="212"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>